<commit_message>
In the middle of Joannas edits
</commit_message>
<xml_diff>
--- a/Tables/Table 1 - Network GO Terms.xlsx
+++ b/Tables/Table 1 - Network GO Terms.xlsx
@@ -72,26 +72,53 @@
     <t>626 (58%)</t>
   </si>
   <si>
-    <t>Number Significant (p&lt;0.01) GO Terms (n=1078)</t>
-  </si>
-  <si>
     <t>Both Scores</t>
   </si>
   <si>
     <t>Either Score</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Number Significant (p </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>≤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 0.01) GO Terms (n = 1078)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -280,15 +307,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -313,6 +331,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -598,7 +625,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,77 +636,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="2"/>
+      <c r="B1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -688,5 +715,6 @@
     <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>